<commit_message>
Sync: Export program data - 2025-09-24T15:48:28.308Z
</commit_message>
<xml_diff>
--- a/master-data/program-portfolio.xlsx
+++ b/master-data/program-portfolio.xlsx
@@ -5357,7 +5357,7 @@
         <v>45923.12882056713</v>
       </c>
       <c r="J2" s="1">
-        <v>45923.12882056713</v>
+        <v>45924.65744005787</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
@@ -5389,7 +5389,7 @@
         <v>45923.124348032405</v>
       </c>
       <c r="J3" s="1">
-        <v>45923.124348032405</v>
+        <v>45924.65744091435</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
@@ -5421,7 +5421,7 @@
         <v>45923.12092271991</v>
       </c>
       <c r="J4" s="1">
-        <v>45923.12092271991</v>
+        <v>45924.657441585645</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
@@ -5453,7 +5453,7 @@
         <v>45923.12092271991</v>
       </c>
       <c r="J5" s="1">
-        <v>45923.12092271991</v>
+        <v>45924.65744228009</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
@@ -5485,7 +5485,7 @@
         <v>45923.12092271991</v>
       </c>
       <c r="J6" s="1">
-        <v>45923.12092271991</v>
+        <v>45924.65744297454</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
@@ -5517,7 +5517,7 @@
         <v>45923.12092271991</v>
       </c>
       <c r="J7" s="1">
-        <v>45923.12092271991</v>
+        <v>45924.65744364583</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
@@ -5549,7 +5549,7 @@
         <v>45923.12092271991</v>
       </c>
       <c r="J8" s="1">
-        <v>45923.12092271991</v>
+        <v>45924.6574443287</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
@@ -5581,7 +5581,7 @@
         <v>45923.12063535879</v>
       </c>
       <c r="J9" s="1">
-        <v>45923.12063535879</v>
+        <v>45924.65744502315</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Sync: Export program data - 2025-09-24T15:55:08.966Z
</commit_message>
<xml_diff>
--- a/master-data/program-portfolio.xlsx
+++ b/master-data/program-portfolio.xlsx
@@ -5357,7 +5357,7 @@
         <v>45923.12882056713</v>
       </c>
       <c r="J2" s="1">
-        <v>45924.65744005787</v>
+        <v>45924.6589990162</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
@@ -5389,7 +5389,7 @@
         <v>45923.124348032405</v>
       </c>
       <c r="J3" s="1">
-        <v>45924.65744091435</v>
+        <v>45924.65899972222</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
@@ -5421,7 +5421,7 @@
         <v>45923.12092271991</v>
       </c>
       <c r="J4" s="1">
-        <v>45924.657441585645</v>
+        <v>45924.65900046296</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
@@ -5453,7 +5453,7 @@
         <v>45923.12092271991</v>
       </c>
       <c r="J5" s="1">
-        <v>45924.65744228009</v>
+        <v>45924.65900114583</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
@@ -5485,7 +5485,7 @@
         <v>45923.12092271991</v>
       </c>
       <c r="J6" s="1">
-        <v>45924.65744297454</v>
+        <v>45924.65900181713</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
@@ -5517,7 +5517,7 @@
         <v>45923.12092271991</v>
       </c>
       <c r="J7" s="1">
-        <v>45924.65744364583</v>
+        <v>45924.65900252315</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
@@ -5549,7 +5549,7 @@
         <v>45923.12092271991</v>
       </c>
       <c r="J8" s="1">
-        <v>45924.6574443287</v>
+        <v>45924.65900319444</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
@@ -5581,7 +5581,7 @@
         <v>45923.12063535879</v>
       </c>
       <c r="J9" s="1">
-        <v>45924.65744502315</v>
+        <v>45924.659003877314</v>
       </c>
     </row>
   </sheetData>

</xml_diff>